<commit_message>
select phenotypes for k-mer analysis
</commit_message>
<xml_diff>
--- a/Kmer/output/select-pheno-20220522.xlsx
+++ b/Kmer/output/select-pheno-20220522.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wendy/Documents/CADVIP/Kmer/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABC66A2-40B4-0B40-B8E3-79EA459ADB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF683A35-492D-4E40-B8C9-0104C3AB7A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="660" windowWidth="21580" windowHeight="12760" xr2:uid="{519B33A3-9A9A-4143-BEDE-42514FEC41F0}"/>
+    <workbookView xWindow="1580" yWindow="660" windowWidth="21580" windowHeight="12760" activeTab="1" xr2:uid="{519B33A3-9A9A-4143-BEDE-42514FEC41F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -377,15 +378,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,471 +701,563 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8941B2D5-FD5B-9E45-8C3F-715B4C14F093}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2.2E-16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D82A5D-785D-9146-A7FB-63251DC9D6AA}">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="4">
-        <v>2.2E-16</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="G5" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="G6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="G7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B40" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D42" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A41"/>
-    <mergeCell ref="D2:D41"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>